<commit_message>
updated database.xlsx, corrected Barcelona, Aliga Izmir and Klaipeda lat & lon
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julik\PycharmProjects]\SERTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1AED697-626F-4909-9634-8E2D9B29879C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C582B8-92AD-4659-8C50-BF34C464CF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="193">
   <si>
     <t>country</t>
   </si>
@@ -55,6 +55,9 @@
     <t>Belgium</t>
   </si>
   <si>
+    <t>LNG terminal Zeebrugge</t>
+  </si>
+  <si>
     <t>Zeebrugge</t>
   </si>
   <si>
@@ -73,6 +76,9 @@
     <t>Croatia</t>
   </si>
   <si>
+    <t>LNG Terminal Krk Island</t>
+  </si>
+  <si>
     <t>Krk Island</t>
   </si>
   <si>
@@ -85,36 +91,45 @@
     <t>France</t>
   </si>
   <si>
-    <t>Dunkerque LNG</t>
+    <t>Dunkerque LNG terminal</t>
+  </si>
+  <si>
+    <t>Dunkerque</t>
   </si>
   <si>
     <t>dunkerque LNG</t>
   </si>
   <si>
+    <t>Fos Cavaou LNG terminal</t>
+  </si>
+  <si>
     <t>Fos Cavaou</t>
   </si>
   <si>
     <t>fosmax LNG</t>
   </si>
   <si>
-    <t>expansion 1</t>
-  </si>
-  <si>
-    <t>expansion 2</t>
-  </si>
-  <si>
-    <t>Fos Tonkin</t>
+    <t>Fos Tonkin LNG terminal</t>
+  </si>
+  <si>
+    <t>Fos-sur-Mer</t>
   </si>
   <si>
     <t>elengy</t>
   </si>
   <si>
+    <t>Montoir LNG terminal</t>
+  </si>
+  <si>
     <t>Montoir de Bretagne</t>
   </si>
   <si>
     <t>Greece</t>
   </si>
   <si>
+    <t>Revithoussa LNG terminal</t>
+  </si>
+  <si>
     <t>Revithoussa</t>
   </si>
   <si>
@@ -145,12 +160,18 @@
     <t>possible expension</t>
   </si>
   <si>
+    <t>Panigaglia LNG terminal</t>
+  </si>
+  <si>
     <t>Panigaglia</t>
   </si>
   <si>
     <t>snam</t>
   </si>
   <si>
+    <t>Rovigo LNG terminal</t>
+  </si>
+  <si>
     <t>Rovigo</t>
   </si>
   <si>
@@ -163,7 +184,10 @@
     <t>Lithuania</t>
   </si>
   <si>
-    <t>Independence</t>
+    <t>FSRU Independence</t>
+  </si>
+  <si>
+    <t>Klaipeda</t>
   </si>
   <si>
     <t>KN</t>
@@ -172,6 +196,9 @@
     <t>Malta</t>
   </si>
   <si>
+    <t>Delimara LNG terminal</t>
+  </si>
+  <si>
     <t>Delimara</t>
   </si>
   <si>
@@ -196,9 +223,15 @@
     <t>EemsEnergyTerminal</t>
   </si>
   <si>
+    <t>Groningen</t>
+  </si>
+  <si>
     <t>Poland</t>
   </si>
   <si>
+    <t>Świnoujście LNG terminal</t>
+  </si>
+  <si>
     <t>Świnoujście</t>
   </si>
   <si>
@@ -208,6 +241,9 @@
     <t>Portugal</t>
   </si>
   <si>
+    <t>Sines LNG terminal</t>
+  </si>
+  <si>
     <t>Sines</t>
   </si>
   <si>
@@ -217,6 +253,9 @@
     <t>Russia</t>
   </si>
   <si>
+    <t>Kaliningrad LNG terminal</t>
+  </si>
+  <si>
     <t>Kaliningrad</t>
   </si>
   <si>
@@ -226,33 +265,54 @@
     <t>Spain</t>
   </si>
   <si>
+    <t>Barcelona LNG terminal</t>
+  </si>
+  <si>
     <t>Barcelona</t>
   </si>
   <si>
     <t>enagas</t>
   </si>
   <si>
+    <t>Bilbao LNG terminal</t>
+  </si>
+  <si>
     <t>Bilbao</t>
   </si>
   <si>
     <t>BBG</t>
   </si>
   <si>
+    <t>Cartagena LNG terminal</t>
+  </si>
+  <si>
     <t>Cartagena</t>
   </si>
   <si>
+    <t>El Musel LNG terminal</t>
+  </si>
+  <si>
     <t>Gijón (Musel)</t>
   </si>
   <si>
+    <t>Huelva LNG terminal</t>
+  </si>
+  <si>
     <t>Huelva</t>
   </si>
   <si>
+    <t>Mugardos LNG terminal</t>
+  </si>
+  <si>
     <t>Mugardos</t>
   </si>
   <si>
     <t>reganosa</t>
   </si>
   <si>
+    <t>Sagunto LNG terminal</t>
+  </si>
+  <si>
     <t>Sagunto</t>
   </si>
   <si>
@@ -262,30 +322,45 @@
     <t>Turkey</t>
   </si>
   <si>
+    <t>Aliga Etki LNG terminal</t>
+  </si>
+  <si>
     <t>Aliga Etki</t>
   </si>
   <si>
     <t>etklliman</t>
   </si>
   <si>
+    <t>Aliga Izmir LNG terminal</t>
+  </si>
+  <si>
     <t>Aliga Izmir</t>
   </si>
   <si>
     <t>EgeGaz</t>
   </si>
   <si>
+    <t>Dörtyol LNG terminal</t>
+  </si>
+  <si>
     <t>Dörtyol</t>
   </si>
   <si>
     <t>botgas</t>
   </si>
   <si>
+    <t>Marmara Ereglisi LNG terminal</t>
+  </si>
+  <si>
     <t>Marmara Ereglisi</t>
   </si>
   <si>
     <t>United Kingdom</t>
   </si>
   <si>
+    <t>Grain LNG terminal</t>
+  </si>
+  <si>
     <t>Isle of Grain</t>
   </si>
   <si>
@@ -307,12 +382,18 @@
     <t>Cyprus</t>
   </si>
   <si>
+    <t>Vasiliko LNG terminal</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vasiliko </t>
   </si>
   <si>
     <t>ETYFA</t>
   </si>
   <si>
+    <t>Alexandroupolis LNG terminal</t>
+  </si>
+  <si>
     <t>Alexandroupolis</t>
   </si>
   <si>
@@ -322,6 +403,9 @@
     <t>Albania</t>
   </si>
   <si>
+    <t>Vlora LNG terminal</t>
+  </si>
+  <si>
     <t>Vlora</t>
   </si>
   <si>
@@ -334,12 +418,18 @@
     <t>Estonia</t>
   </si>
   <si>
+    <t>Paldiski LNG terminal</t>
+  </si>
+  <si>
     <t>Paldiski</t>
   </si>
   <si>
     <t>Alexela</t>
   </si>
   <si>
+    <t>Tallinn LNG terminal</t>
+  </si>
+  <si>
     <t>Tallinn (Muuga)</t>
   </si>
   <si>
@@ -352,9 +442,15 @@
     <t>Exemplar FSRU</t>
   </si>
   <si>
+    <t>Inkoo</t>
+  </si>
+  <si>
     <t>gasgrid fortum</t>
   </si>
   <si>
+    <t>Le Havre LNG terminal</t>
+  </si>
+  <si>
     <t>Le Havre</t>
   </si>
   <si>
@@ -364,24 +460,36 @@
     <t>Germany</t>
   </si>
   <si>
+    <t>Brunsbüttel LNG terminal</t>
+  </si>
+  <si>
     <t>Brunsbüttel</t>
   </si>
   <si>
     <t>gasunte</t>
   </si>
   <si>
+    <t>Lubmin LNG terminal</t>
+  </si>
+  <si>
     <t>Lubmin</t>
   </si>
   <si>
     <t>deutsche RaGas</t>
   </si>
   <si>
+    <t>Stade LNG terminal</t>
+  </si>
+  <si>
     <t>Stade</t>
   </si>
   <si>
     <t>Hanseatic Energy Hub</t>
   </si>
   <si>
+    <t>Wilhelmshaven LNG terminal</t>
+  </si>
+  <si>
     <t>Wilhelmshaven</t>
   </si>
   <si>
@@ -391,19 +499,25 @@
     <t>TES</t>
   </si>
   <si>
+    <t>Argo LNG terminal</t>
+  </si>
+  <si>
     <t>Argo</t>
   </si>
   <si>
     <t>Mediterranean Gas</t>
   </si>
   <si>
-    <t>Dioriga Gas (Corynth)</t>
+    <t>Dioriga FSRU</t>
+  </si>
+  <si>
+    <t>Gulf of Corinth</t>
   </si>
   <si>
     <t>Gioriga Gas</t>
   </si>
   <si>
-    <t>Thrace LNG Terminal</t>
+    <t>Thrace  FSRU</t>
   </si>
   <si>
     <t>gas trade</t>
@@ -415,19 +529,34 @@
     <t>Shannon LNG</t>
   </si>
   <si>
+    <t>Tarbert/Ballylongford</t>
+  </si>
+  <si>
     <t>shannon LNG</t>
   </si>
   <si>
-    <t>Mag Mell</t>
+    <t>Mag Mell FSRU</t>
+  </si>
+  <si>
+    <t>Cork</t>
   </si>
   <si>
     <t xml:space="preserve">Mag Mell </t>
   </si>
   <si>
-    <t>FSRU 1 - SNAM</t>
-  </si>
-  <si>
-    <t>FSRU 2 - SNAM</t>
+    <t>Porto Torres FSRU</t>
+  </si>
+  <si>
+    <t>Porto Torres</t>
+  </si>
+  <si>
+    <t>Die Schiffe werden zwischen den Regasifizierungsterminals von Panigaglia (La Spezia) und Olt (Livorno) in Richtung der Fsru-Einheit pendeln, die im Industriehafen von Porto Torres installiert ist,</t>
+  </si>
+  <si>
+    <t>Ravenna FSRU</t>
+  </si>
+  <si>
+    <t>Ravenna</t>
   </si>
   <si>
     <t>Porto Empedoche</t>
@@ -460,7 +589,13 @@
     <t>Gdansk LNG</t>
   </si>
   <si>
+    <t>Gdansk</t>
+  </si>
+  <si>
     <t>GAZ system</t>
+  </si>
+  <si>
+    <t>Gulf of Saros FSRU</t>
   </si>
   <si>
     <t>Gulf of Saros</t>
@@ -474,7 +609,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,13 +623,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11.5"/>
       <color rgb="FF212529"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.5"/>
-      <color rgb="FF5F6368"/>
+      <sz val="12"/>
+      <color indexed="64"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -504,7 +645,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -517,6 +658,12 @@
         <bgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -527,29 +674,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -784,7 +936,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="5" width="18.109375" customWidth="1"/>
     <col min="6" max="6" width="27.44140625" bestFit="1" customWidth="1"/>
@@ -824,12 +977,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="13.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1">
         <v>3.22241</v>
@@ -838,13 +994,13 @@
         <v>51.353000000000002</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="2">
         <v>11400000000</v>
@@ -857,8 +1013,11 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1">
         <v>3.22241</v>
@@ -867,13 +1026,13 @@
         <v>51.353000000000002</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
         <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
       </c>
       <c r="I3" s="2">
         <v>3900000000</v>
@@ -886,8 +1045,11 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1">
         <v>3.22241</v>
@@ -896,13 +1058,13 @@
         <v>51.353000000000002</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
         <v>15</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
       </c>
       <c r="I4" s="2">
         <v>1800000000</v>
@@ -913,10 +1075,13 @@
     </row>
     <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1">
         <v>14.6</v>
@@ -925,13 +1090,13 @@
         <v>45.066667000000002</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I5" s="2">
         <v>2600000000</v>
@@ -942,10 +1107,13 @@
     </row>
     <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1">
         <v>14.6</v>
@@ -954,13 +1122,13 @@
         <v>45.066668</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I6" s="2">
         <v>2600000000</v>
@@ -969,27 +1137,30 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="3">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1">
         <v>2.1965300000000001</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>51.033610000000003</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I7" s="2">
         <v>13000000000</v>
@@ -1000,10 +1171,13 @@
     </row>
     <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1">
         <v>4.9010199999999999</v>
@@ -1012,13 +1186,13 @@
         <v>43.419629999999998</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I8" s="2">
         <v>8500000000</v>
@@ -1029,10 +1203,13 @@
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D9" s="1">
         <v>4.9010199999999999</v>
@@ -1041,13 +1218,13 @@
         <v>43.419629999999998</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H9" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I9" s="2">
         <v>1500000000</v>
@@ -1058,10 +1235,13 @@
     </row>
     <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1">
         <v>4.9010199999999999</v>
@@ -1070,13 +1250,13 @@
         <v>43.419629999999998</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I10" s="2">
         <v>2000000000</v>
@@ -1087,10 +1267,13 @@
     </row>
     <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1">
         <v>4.9010199999999999</v>
@@ -1099,13 +1282,13 @@
         <v>43.419629999999998</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H11" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I11" s="2">
         <v>1500000000</v>
@@ -1116,10 +1299,13 @@
     </row>
     <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D12" s="1">
         <v>-2.1427800000000001</v>
@@ -1128,13 +1314,13 @@
         <v>47.302959999999999</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H12" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I12" s="2">
         <v>10000000000</v>
@@ -1145,25 +1331,28 @@
     </row>
     <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1">
         <v>23.4023</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H13" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="I13" s="2">
         <v>7000000000</v>
@@ -1174,28 +1363,28 @@
     </row>
     <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E14" s="1">
         <v>43.644444</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H14" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="I14" s="2">
         <v>3550000000</v>
@@ -1206,28 +1395,28 @@
     </row>
     <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E15" s="1">
         <v>43.644444999999997</v>
       </c>
       <c r="F15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="I15" s="2">
         <v>1190000000</v>
@@ -1236,15 +1425,18 @@
         <v>2013</v>
       </c>
       <c r="K15" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D16" s="1">
         <v>9.8308700000000009</v>
@@ -1253,13 +1445,13 @@
         <v>44.074280000000002</v>
       </c>
       <c r="F16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H16" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="I16" s="2">
         <v>3400000000</v>
@@ -1270,10 +1462,13 @@
     </row>
     <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D17" s="1">
         <v>12.586111000000001</v>
@@ -1282,13 +1477,13 @@
         <v>45.091667000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="G17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H17" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="I17" s="2">
         <v>9000000000</v>
@@ -1299,10 +1494,13 @@
     </row>
     <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D18" s="1">
         <v>21.137619999999998</v>
@@ -1311,13 +1509,13 @@
         <v>55.66451</v>
       </c>
       <c r="F18" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H18" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="I18" s="2">
         <v>4000000000</v>
@@ -1328,10 +1526,13 @@
     </row>
     <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D19" s="1">
         <v>14.5542</v>
@@ -1340,13 +1541,13 @@
         <v>35.8277</v>
       </c>
       <c r="F19" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="G19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H19" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="I19" s="2">
         <v>700000000</v>
@@ -1357,13 +1558,13 @@
     </row>
     <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D20" s="1">
         <v>4.0688890000000004</v>
@@ -1372,13 +1573,13 @@
         <v>51.971111000000001</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H20" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="I20" s="2">
         <v>12000000000</v>
@@ -1389,13 +1590,13 @@
     </row>
     <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D21" s="1">
         <v>4.0688890000000004</v>
@@ -1404,13 +1605,13 @@
         <v>51.971111000000001</v>
       </c>
       <c r="F21" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="G21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H21" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="I21" s="2">
         <v>4000000000</v>
@@ -1418,16 +1619,19 @@
       <c r="J21">
         <v>2011</v>
       </c>
+      <c r="K21" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D22" s="1">
         <v>4.0688890000000004</v>
@@ -1436,13 +1640,13 @@
         <v>51.971111000000001</v>
       </c>
       <c r="F22" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="G22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H22" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="I22" s="2">
         <v>1500000000</v>
@@ -1453,13 +1657,13 @@
     </row>
     <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D23" s="1">
         <v>4.0688890000000004</v>
@@ -1468,13 +1672,13 @@
         <v>51.971111000000001</v>
       </c>
       <c r="F23" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="G23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H23" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="I23" s="2">
         <v>2500000000</v>
@@ -1485,13 +1689,13 @@
     </row>
     <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="D24" s="1">
         <v>6.8330976999999997</v>
@@ -1500,13 +1704,13 @@
         <v>53.435648700000002</v>
       </c>
       <c r="F24" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H24" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="I24" s="2">
         <v>8000000000</v>
@@ -1517,10 +1721,13 @@
     </row>
     <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
+        <v>69</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="D25" s="1">
         <v>14.294722</v>
@@ -1529,13 +1736,13 @@
         <v>53.909166999999997</v>
       </c>
       <c r="F25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H25" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="I25" s="2">
         <v>6200000000</v>
@@ -1546,10 +1753,13 @@
     </row>
     <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>68</v>
+      </c>
+      <c r="B26" t="s">
+        <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="D26" s="1">
         <v>14.294722</v>
@@ -1558,13 +1768,13 @@
         <v>53.909166999999997</v>
       </c>
       <c r="F26" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="G26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H26" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="I26" s="2">
         <v>2100000000</v>
@@ -1575,10 +1785,13 @@
     </row>
     <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>72</v>
+      </c>
+      <c r="B27" t="s">
+        <v>73</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="D27" s="1">
         <v>-8.8435000000000006</v>
@@ -1587,13 +1800,13 @@
         <v>37.941899999999997</v>
       </c>
       <c r="F27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H27" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="I27" s="2">
         <v>7600000000</v>
@@ -1603,41 +1816,46 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" s="5">
+      <c r="A28" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="4">
         <v>20.362926099999999</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="4">
         <v>54.983699899999998</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="I28" s="6">
+      <c r="F28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I28" s="5">
         <v>3700000000</v>
       </c>
-      <c r="J28" s="4">
+      <c r="J28" s="3">
         <v>2019</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>80</v>
+      </c>
+      <c r="B29" t="s">
+        <v>81</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="D29" s="1">
         <v>2.1583000000000001</v>
@@ -1646,13 +1864,13 @@
         <v>41.339399999999998</v>
       </c>
       <c r="F29" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H29" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="I29" s="2">
         <v>17100000000</v>
@@ -1663,10 +1881,13 @@
     </row>
     <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>80</v>
+      </c>
+      <c r="B30" t="s">
+        <v>84</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="D30" s="1">
         <v>-3.0947300000000002</v>
@@ -1675,13 +1896,13 @@
         <v>43.361199999999997</v>
       </c>
       <c r="F30" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H30" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="I30" s="2">
         <v>7000000000</v>
@@ -1692,10 +1913,13 @@
     </row>
     <row r="31" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>80</v>
+      </c>
+      <c r="B31" t="s">
+        <v>87</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="D31" s="1">
         <v>-0.95950000000000002</v>
@@ -1704,13 +1928,13 @@
         <v>37.574570000000001</v>
       </c>
       <c r="F31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H31" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="I31" s="2">
         <v>11800000000</v>
@@ -1721,10 +1945,13 @@
     </row>
     <row r="32" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>80</v>
+      </c>
+      <c r="B32" t="s">
+        <v>89</v>
       </c>
       <c r="C32" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="D32" s="1">
         <v>-5.6933999999999996</v>
@@ -1733,13 +1960,13 @@
         <v>43.569600000000001</v>
       </c>
       <c r="F32" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H32" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="I32" s="2">
         <v>7000000000</v>
@@ -1753,10 +1980,13 @@
     </row>
     <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>80</v>
+      </c>
+      <c r="B33" t="s">
+        <v>91</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="D33" s="1">
         <v>-6.9109999999999996</v>
@@ -1765,13 +1995,13 @@
         <v>37.173549999999999</v>
       </c>
       <c r="F33" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H33" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="I33" s="2">
         <v>11800000000</v>
@@ -1782,10 +2012,13 @@
     </row>
     <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>80</v>
+      </c>
+      <c r="B34" t="s">
+        <v>93</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="D34" s="1">
         <v>-8.2394999999999996</v>
@@ -1794,15 +2027,15 @@
         <v>43.461300000000001</v>
       </c>
       <c r="F34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H34" t="s">
-        <v>76</v>
-      </c>
-      <c r="I34" s="7">
+        <v>95</v>
+      </c>
+      <c r="I34" s="6">
         <v>3600000000</v>
       </c>
       <c r="J34">
@@ -1811,10 +2044,13 @@
     </row>
     <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>80</v>
+      </c>
+      <c r="B35" t="s">
+        <v>96</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="D35" s="1">
         <v>-0.2152</v>
@@ -1823,15 +2059,15 @@
         <v>39.632899999999999</v>
       </c>
       <c r="F35" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H35" t="s">
-        <v>78</v>
-      </c>
-      <c r="I35" s="7">
+        <v>98</v>
+      </c>
+      <c r="I35" s="6">
         <v>8800000000</v>
       </c>
       <c r="J35">
@@ -1840,10 +2076,13 @@
     </row>
     <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>99</v>
+      </c>
+      <c r="B36" t="s">
+        <v>100</v>
       </c>
       <c r="C36" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="D36" s="1">
         <v>27.129000000000001</v>
@@ -1852,15 +2091,15 @@
         <v>38.421999999999997</v>
       </c>
       <c r="F36" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H36" t="s">
-        <v>81</v>
-      </c>
-      <c r="I36" s="7">
+        <v>102</v>
+      </c>
+      <c r="I36" s="6">
         <v>7300000000</v>
       </c>
       <c r="J36">
@@ -1869,27 +2108,30 @@
     </row>
     <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>99</v>
+      </c>
+      <c r="B37" t="s">
+        <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="D37" s="1">
+        <v>26.970278</v>
+      </c>
+      <c r="E37" s="1">
         <v>38.795000000000002</v>
       </c>
-      <c r="E37" s="1">
-        <v>26.970278</v>
-      </c>
       <c r="F37" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H37" t="s">
-        <v>83</v>
-      </c>
-      <c r="I37" s="7">
+        <v>105</v>
+      </c>
+      <c r="I37" s="6">
         <v>13800000000</v>
       </c>
       <c r="J37">
@@ -1898,10 +2140,13 @@
     </row>
     <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>99</v>
+      </c>
+      <c r="B38" t="s">
+        <v>106</v>
       </c>
       <c r="C38" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="D38" s="1">
         <v>36.131414700000001</v>
@@ -1910,15 +2155,15 @@
         <v>36.855579300000002</v>
       </c>
       <c r="F38" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H38" t="s">
-        <v>85</v>
-      </c>
-      <c r="I38" s="7">
+        <v>108</v>
+      </c>
+      <c r="I38" s="6">
         <v>9700000000</v>
       </c>
       <c r="J38">
@@ -1927,10 +2172,13 @@
     </row>
     <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>79</v>
+        <v>99</v>
+      </c>
+      <c r="B39" t="s">
+        <v>109</v>
       </c>
       <c r="C39" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="D39" s="1">
         <v>27.955278</v>
@@ -1939,15 +2187,15 @@
         <v>40.969721999999997</v>
       </c>
       <c r="F39" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H39" t="s">
-        <v>85</v>
-      </c>
-      <c r="I39" s="7">
+        <v>108</v>
+      </c>
+      <c r="I39" s="6">
         <v>12800000000</v>
       </c>
       <c r="J39">
@@ -1956,10 +2204,13 @@
     </row>
     <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>111</v>
+      </c>
+      <c r="B40" t="s">
+        <v>112</v>
       </c>
       <c r="C40" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="D40" s="1">
         <v>0.67986999999999997</v>
@@ -1968,15 +2219,15 @@
         <v>51.451070000000001</v>
       </c>
       <c r="F40" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H40" t="s">
-        <v>89</v>
-      </c>
-      <c r="I40" s="7">
+        <v>114</v>
+      </c>
+      <c r="I40" s="6">
         <v>19500000000</v>
       </c>
       <c r="J40">
@@ -1985,10 +2236,13 @@
     </row>
     <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>111</v>
+      </c>
+      <c r="B41" t="s">
+        <v>112</v>
       </c>
       <c r="C41" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="D41" s="1">
         <v>0.67986999999999997</v>
@@ -1997,15 +2251,15 @@
         <v>51.451070000000001</v>
       </c>
       <c r="F41" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G41" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H41" t="s">
-        <v>89</v>
-      </c>
-      <c r="I41" s="7">
+        <v>114</v>
+      </c>
+      <c r="I41" s="6">
         <v>5000000000</v>
       </c>
       <c r="J41">
@@ -2014,10 +2268,13 @@
     </row>
     <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>111</v>
+      </c>
+      <c r="B42" t="s">
+        <v>115</v>
       </c>
       <c r="C42" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="D42" s="1">
         <v>-4.9977400000000003</v>
@@ -2026,15 +2283,15 @@
         <v>51.704529999999998</v>
       </c>
       <c r="F42" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H42" t="s">
-        <v>91</v>
-      </c>
-      <c r="I42" s="7">
+        <v>116</v>
+      </c>
+      <c r="I42" s="6">
         <v>7600000000</v>
       </c>
       <c r="J42">
@@ -2043,10 +2300,13 @@
     </row>
     <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>111</v>
+      </c>
+      <c r="B43" t="s">
+        <v>117</v>
       </c>
       <c r="C43" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="D43" s="1">
         <v>-4.9977400000000003</v>
@@ -2055,15 +2315,15 @@
         <v>51.704529999999998</v>
       </c>
       <c r="F43" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H43" t="s">
-        <v>93</v>
-      </c>
-      <c r="I43" s="7">
+        <v>118</v>
+      </c>
+      <c r="I43" s="6">
         <v>21000000000</v>
       </c>
       <c r="J43">
@@ -2072,10 +2332,13 @@
     </row>
     <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>94</v>
+        <v>119</v>
+      </c>
+      <c r="B44" t="s">
+        <v>120</v>
       </c>
       <c r="C44" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="D44" s="1">
         <v>33.30104</v>
@@ -2084,15 +2347,15 @@
         <v>34.727719999999998</v>
       </c>
       <c r="F44" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H44" t="s">
-        <v>96</v>
-      </c>
-      <c r="I44" s="7">
+        <v>122</v>
+      </c>
+      <c r="I44" s="6">
         <v>2440000000</v>
       </c>
       <c r="J44">
@@ -2101,10 +2364,13 @@
     </row>
     <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="B45" t="s">
+        <v>123</v>
       </c>
       <c r="C45" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="D45" s="1">
         <v>25.842735999999999</v>
@@ -2113,15 +2379,15 @@
         <v>40.774729999999998</v>
       </c>
       <c r="F45" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H45" t="s">
-        <v>98</v>
-      </c>
-      <c r="I45" s="7">
+        <v>125</v>
+      </c>
+      <c r="I45" s="6">
         <v>5500000000</v>
       </c>
       <c r="J45">
@@ -2130,10 +2396,13 @@
     </row>
     <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>99</v>
+        <v>126</v>
+      </c>
+      <c r="B46" t="s">
+        <v>127</v>
       </c>
       <c r="C46" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="D46" s="1">
         <v>19.480761000000001</v>
@@ -2142,16 +2411,16 @@
         <v>40.449271000000003</v>
       </c>
       <c r="F46" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H46" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="I46" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="J46">
         <v>2023</v>
@@ -2159,10 +2428,13 @@
     </row>
     <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>103</v>
+        <v>131</v>
+      </c>
+      <c r="B47" t="s">
+        <v>132</v>
       </c>
       <c r="C47" t="s">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="D47" s="1">
         <v>24.074940000000002</v>
@@ -2171,15 +2443,15 @@
         <v>59.384450000000001</v>
       </c>
       <c r="F47" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H47" t="s">
-        <v>105</v>
-      </c>
-      <c r="I47" s="7">
+        <v>134</v>
+      </c>
+      <c r="I47" s="6">
         <v>2500000000</v>
       </c>
       <c r="J47">
@@ -2188,10 +2460,13 @@
     </row>
     <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>103</v>
+        <v>131</v>
+      </c>
+      <c r="B48" t="s">
+        <v>135</v>
       </c>
       <c r="C48" t="s">
-        <v>106</v>
+        <v>136</v>
       </c>
       <c r="D48" s="1">
         <v>25.0045</v>
@@ -2200,50 +2475,62 @@
         <v>59.506010000000003</v>
       </c>
       <c r="F48" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H48" t="s">
-        <v>107</v>
-      </c>
-      <c r="I48" s="7">
+        <v>137</v>
+      </c>
+      <c r="I48" s="6">
         <v>4000000000</v>
       </c>
       <c r="J48" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>108</v>
+        <v>138</v>
+      </c>
+      <c r="B49" t="s">
+        <v>139</v>
       </c>
       <c r="C49" t="s">
-        <v>109</v>
+        <v>140</v>
+      </c>
+      <c r="D49" s="1">
+        <v>24.006440999999999</v>
+      </c>
+      <c r="E49" s="1">
+        <v>60.041103</v>
       </c>
       <c r="F49" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H49" t="s">
-        <v>110</v>
-      </c>
-      <c r="I49" s="7">
+        <v>141</v>
+      </c>
+      <c r="I49" s="6">
         <v>5000000000</v>
       </c>
       <c r="J49">
         <v>2023</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="B50" t="s">
+        <v>142</v>
       </c>
       <c r="C50" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="D50" s="1">
         <v>4.2958425760000002E-2</v>
@@ -2252,27 +2539,30 @@
         <v>49.462228393267502</v>
       </c>
       <c r="F50" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G50" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H50" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="I50" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="J50" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>113</v>
+        <v>145</v>
+      </c>
+      <c r="B51" t="s">
+        <v>146</v>
       </c>
       <c r="C51" t="s">
-        <v>114</v>
+        <v>147</v>
       </c>
       <c r="D51" s="1">
         <v>8.9760945000000003</v>
@@ -2281,27 +2571,30 @@
         <v>53.914000899999998</v>
       </c>
       <c r="F51" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H51" t="s">
-        <v>115</v>
-      </c>
-      <c r="I51" s="7">
+        <v>148</v>
+      </c>
+      <c r="I51" s="6">
         <v>5000000000</v>
       </c>
       <c r="J51">
         <v>2023</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>113</v>
+        <v>145</v>
+      </c>
+      <c r="B52" t="s">
+        <v>149</v>
       </c>
       <c r="C52" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="D52" s="1">
         <v>13.645319000000001</v>
@@ -2310,27 +2603,30 @@
         <v>54.153331999999999</v>
       </c>
       <c r="F52" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G52" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H52" t="s">
-        <v>117</v>
-      </c>
-      <c r="I52" s="7">
+        <v>151</v>
+      </c>
+      <c r="I52" s="6">
         <v>4500000000</v>
       </c>
       <c r="J52">
         <v>2023</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>113</v>
+        <v>145</v>
+      </c>
+      <c r="B53" t="s">
+        <v>152</v>
       </c>
       <c r="C53" t="s">
-        <v>118</v>
+        <v>153</v>
       </c>
       <c r="D53" s="1">
         <v>9.5103819999999999</v>
@@ -2339,27 +2635,30 @@
         <v>53.652459</v>
       </c>
       <c r="F53" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G53" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H53" t="s">
-        <v>119</v>
-      </c>
-      <c r="I53" s="7">
+        <v>154</v>
+      </c>
+      <c r="I53" s="6">
         <v>12000000000</v>
       </c>
       <c r="J53">
         <v>2026</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>113</v>
+        <v>145</v>
+      </c>
+      <c r="B54" t="s">
+        <v>155</v>
       </c>
       <c r="C54" t="s">
-        <v>120</v>
+        <v>156</v>
       </c>
       <c r="D54" s="1">
         <v>8.1333330000000004</v>
@@ -2368,27 +2667,30 @@
         <v>53.516666999999998</v>
       </c>
       <c r="F54" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H54" t="s">
-        <v>121</v>
-      </c>
-      <c r="I54" s="7">
+        <v>157</v>
+      </c>
+      <c r="I54" s="6">
         <v>7500000000</v>
       </c>
       <c r="J54">
         <v>2023</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>113</v>
+        <v>145</v>
+      </c>
+      <c r="B55" t="s">
+        <v>155</v>
       </c>
       <c r="C55" t="s">
-        <v>120</v>
+        <v>156</v>
       </c>
       <c r="D55" s="1">
         <v>8.1333330000000004</v>
@@ -2397,27 +2699,30 @@
         <v>53.516666999999998</v>
       </c>
       <c r="F55" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G55" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H55" t="s">
-        <v>122</v>
-      </c>
-      <c r="I55" s="7">
+        <v>158</v>
+      </c>
+      <c r="I55" s="6">
         <v>2200000000</v>
       </c>
       <c r="J55">
         <v>2025</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="B56" t="s">
+        <v>159</v>
       </c>
       <c r="C56" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="D56" s="1">
         <v>22.932490399999999</v>
@@ -2426,27 +2731,30 @@
         <v>39.351264399999998</v>
       </c>
       <c r="F56" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G56" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H56" t="s">
-        <v>124</v>
-      </c>
-      <c r="I56" s="7">
+        <v>161</v>
+      </c>
+      <c r="I56" s="6">
         <v>5200000000</v>
       </c>
       <c r="J56">
         <v>2024</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="B57" t="s">
+        <v>162</v>
       </c>
       <c r="C57" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
       <c r="D57" s="1">
         <v>23.063538999999999</v>
@@ -2455,27 +2763,30 @@
         <v>37.910919999999997</v>
       </c>
       <c r="F57" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H57" t="s">
-        <v>126</v>
-      </c>
-      <c r="I57" s="7">
+        <v>164</v>
+      </c>
+      <c r="I57" s="6">
         <v>3000000000</v>
       </c>
       <c r="J57">
         <v>2026</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="B58" t="s">
+        <v>165</v>
       </c>
       <c r="C58" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D58" s="1">
         <v>25.718754000000001</v>
@@ -2484,27 +2795,30 @@
         <v>40.748353999999999</v>
       </c>
       <c r="F58" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G58" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H58" t="s">
-        <v>128</v>
-      </c>
-      <c r="I58" s="7">
+        <v>166</v>
+      </c>
+      <c r="I58" s="6">
         <v>5500000000</v>
       </c>
       <c r="J58" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>129</v>
+        <v>167</v>
+      </c>
+      <c r="B59" t="s">
+        <v>168</v>
       </c>
       <c r="C59" t="s">
-        <v>130</v>
+        <v>169</v>
       </c>
       <c r="D59" s="1">
         <v>-9.4424600000000005</v>
@@ -2513,27 +2827,30 @@
         <v>52.58099</v>
       </c>
       <c r="F59" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H59" t="s">
-        <v>131</v>
-      </c>
-      <c r="I59" s="7">
+        <v>170</v>
+      </c>
+      <c r="I59" s="6">
         <v>7800000000</v>
       </c>
       <c r="J59" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>129</v>
+        <v>167</v>
+      </c>
+      <c r="B60" t="s">
+        <v>171</v>
       </c>
       <c r="C60" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="D60" s="1">
         <v>-8.0456190000000003</v>
@@ -2542,73 +2859,91 @@
         <v>51.264274</v>
       </c>
       <c r="F60" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G60" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H60" t="s">
-        <v>133</v>
-      </c>
-      <c r="I60" s="7">
+        <v>173</v>
+      </c>
+      <c r="I60" s="6">
         <v>2600000000</v>
       </c>
       <c r="J60">
         <v>2024</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>34</v>
-      </c>
-      <c r="C61" t="s">
-        <v>134</v>
-      </c>
-      <c r="F61" t="s">
-        <v>18</v>
-      </c>
-      <c r="G61" t="s">
-        <v>13</v>
-      </c>
-      <c r="H61" t="s">
-        <v>42</v>
-      </c>
-      <c r="I61" s="7">
+    <row r="61" spans="1:11" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D61" s="8">
+        <v>8.3957188499999997</v>
+      </c>
+      <c r="E61" s="8">
+        <v>40.846639830000001</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H61" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I61" s="9">
         <v>5000000000</v>
       </c>
-      <c r="J61">
+      <c r="J61" s="7">
         <v>2023</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>34</v>
-      </c>
-      <c r="C62" t="s">
-        <v>135</v>
-      </c>
-      <c r="F62" t="s">
-        <v>18</v>
-      </c>
-      <c r="G62" t="s">
-        <v>13</v>
-      </c>
-      <c r="H62" t="s">
-        <v>42</v>
-      </c>
-      <c r="I62" s="7">
+      <c r="K61" s="10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H62" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I62" s="9">
         <v>5000000000</v>
       </c>
-      <c r="J62">
+      <c r="J62" s="7">
         <v>2024</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>34</v>
+        <v>39</v>
+      </c>
+      <c r="B63" t="s">
+        <v>179</v>
       </c>
       <c r="C63" t="s">
-        <v>136</v>
+        <v>179</v>
       </c>
       <c r="D63" s="1">
         <v>13.537739999999999</v>
@@ -2617,27 +2952,30 @@
         <v>37.282969999999999</v>
       </c>
       <c r="F63" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H63" t="s">
-        <v>137</v>
-      </c>
-      <c r="I63" s="7">
+        <v>180</v>
+      </c>
+      <c r="I63" s="6">
         <v>8000000000</v>
       </c>
       <c r="J63">
         <v>2024</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>138</v>
+        <v>181</v>
+      </c>
+      <c r="B64" t="s">
+        <v>182</v>
       </c>
       <c r="C64" t="s">
-        <v>139</v>
+        <v>182</v>
       </c>
       <c r="D64" s="1">
         <v>24.367000000000001</v>
@@ -2646,15 +2984,15 @@
         <v>57.314999999999998</v>
       </c>
       <c r="F64" t="s">
-        <v>140</v>
+        <v>183</v>
       </c>
       <c r="G64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H64" t="s">
-        <v>141</v>
-      </c>
-      <c r="I64" s="7">
+        <v>184</v>
+      </c>
+      <c r="I64" s="6">
         <v>1500000000</v>
       </c>
       <c r="J64">
@@ -2663,10 +3001,13 @@
     </row>
     <row r="65" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>142</v>
+        <v>185</v>
+      </c>
+      <c r="B65" t="s">
+        <v>186</v>
       </c>
       <c r="C65" t="s">
-        <v>143</v>
+        <v>186</v>
       </c>
       <c r="D65" s="1">
         <v>-8.6202799999999993</v>
@@ -2675,32 +3016,35 @@
         <v>33.1267</v>
       </c>
       <c r="F65" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G65" t="s">
-        <v>13</v>
-      </c>
-      <c r="I65" s="7">
+        <v>14</v>
+      </c>
+      <c r="I65" s="6">
         <v>5000000000</v>
       </c>
       <c r="J65" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>142</v>
+        <v>185</v>
+      </c>
+      <c r="B66" t="s">
+        <v>187</v>
       </c>
       <c r="C66" t="s">
-        <v>144</v>
+        <v>187</v>
       </c>
       <c r="F66" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G66" t="s">
-        <v>13</v>
-      </c>
-      <c r="I66" s="7">
+        <v>14</v>
+      </c>
+      <c r="I66" s="6">
         <v>3000000000</v>
       </c>
       <c r="J66">
@@ -2709,10 +3053,13 @@
     </row>
     <row r="67" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>58</v>
+        <v>68</v>
+      </c>
+      <c r="B67" t="s">
+        <v>188</v>
       </c>
       <c r="C67" t="s">
-        <v>145</v>
+        <v>189</v>
       </c>
       <c r="D67" s="1">
         <v>18.716445</v>
@@ -2721,15 +3068,15 @@
         <v>54.407321000000003</v>
       </c>
       <c r="F67" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G67" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H67" t="s">
-        <v>146</v>
-      </c>
-      <c r="I67" s="7">
+        <v>190</v>
+      </c>
+      <c r="I67" s="6">
         <v>6100000000</v>
       </c>
       <c r="J67">
@@ -2738,10 +3085,13 @@
     </row>
     <row r="68" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>79</v>
+        <v>99</v>
+      </c>
+      <c r="B68" t="s">
+        <v>191</v>
       </c>
       <c r="C68" t="s">
-        <v>147</v>
+        <v>192</v>
       </c>
       <c r="D68" s="1">
         <v>26.412033999999998</v>
@@ -2750,9 +3100,9 @@
         <v>40.594648999999997</v>
       </c>
       <c r="F68" t="s">
-        <v>18</v>
-      </c>
-      <c r="I68" s="7">
+        <v>20</v>
+      </c>
+      <c r="I68" s="6">
         <v>9700000000</v>
       </c>
       <c r="J68">

</xml_diff>

<commit_message>
added stats for demand vs capacities
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julik\PycharmProjects]\SERTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C582B8-92AD-4659-8C50-BF34C464CF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BD0A91-3055-4659-925B-8D31F46A8990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="139">
   <si>
     <t>country</t>
   </si>
@@ -55,9 +68,6 @@
     <t>Belgium</t>
   </si>
   <si>
-    <t>LNG terminal Zeebrugge</t>
-  </si>
-  <si>
     <t>Zeebrugge</t>
   </si>
   <si>
@@ -76,9 +86,6 @@
     <t>Croatia</t>
   </si>
   <si>
-    <t>LNG Terminal Krk Island</t>
-  </si>
-  <si>
     <t>Krk Island</t>
   </si>
   <si>
@@ -91,45 +98,30 @@
     <t>France</t>
   </si>
   <si>
-    <t>Dunkerque LNG terminal</t>
-  </si>
-  <si>
-    <t>Dunkerque</t>
+    <t>Dunkerque LNG</t>
   </si>
   <si>
     <t>dunkerque LNG</t>
   </si>
   <si>
-    <t>Fos Cavaou LNG terminal</t>
-  </si>
-  <si>
     <t>Fos Cavaou</t>
   </si>
   <si>
     <t>fosmax LNG</t>
   </si>
   <si>
-    <t>Fos Tonkin LNG terminal</t>
-  </si>
-  <si>
-    <t>Fos-sur-Mer</t>
+    <t>Fos Tonkin</t>
   </si>
   <si>
     <t>elengy</t>
   </si>
   <si>
-    <t>Montoir LNG terminal</t>
-  </si>
-  <si>
     <t>Montoir de Bretagne</t>
   </si>
   <si>
     <t>Greece</t>
   </si>
   <si>
-    <t>Revithoussa LNG terminal</t>
-  </si>
-  <si>
     <t>Revithoussa</t>
   </si>
   <si>
@@ -157,21 +149,12 @@
     <t> 9.988890</t>
   </si>
   <si>
-    <t>possible expension</t>
-  </si>
-  <si>
-    <t>Panigaglia LNG terminal</t>
-  </si>
-  <si>
     <t>Panigaglia</t>
   </si>
   <si>
     <t>snam</t>
   </si>
   <si>
-    <t>Rovigo LNG terminal</t>
-  </si>
-  <si>
     <t>Rovigo</t>
   </si>
   <si>
@@ -184,10 +167,7 @@
     <t>Lithuania</t>
   </si>
   <si>
-    <t>FSRU Independence</t>
-  </si>
-  <si>
-    <t>Klaipeda</t>
+    <t>Independence</t>
   </si>
   <si>
     <t>KN</t>
@@ -196,9 +176,6 @@
     <t>Malta</t>
   </si>
   <si>
-    <t>Delimara LNG terminal</t>
-  </si>
-  <si>
     <t>Delimara</t>
   </si>
   <si>
@@ -217,21 +194,12 @@
     <t>Rotterdam</t>
   </si>
   <si>
-    <t>interrupt</t>
-  </si>
-  <si>
     <t>EemsEnergyTerminal</t>
   </si>
   <si>
-    <t>Groningen</t>
-  </si>
-  <si>
     <t>Poland</t>
   </si>
   <si>
-    <t>Świnoujście LNG terminal</t>
-  </si>
-  <si>
     <t>Świnoujście</t>
   </si>
   <si>
@@ -241,78 +209,42 @@
     <t>Portugal</t>
   </si>
   <si>
-    <t>Sines LNG terminal</t>
-  </si>
-  <si>
     <t>Sines</t>
   </si>
   <si>
     <t>REN Atlântico</t>
   </si>
   <si>
-    <t>Russia</t>
-  </si>
-  <si>
-    <t>Kaliningrad LNG terminal</t>
-  </si>
-  <si>
-    <t>Kaliningrad</t>
-  </si>
-  <si>
-    <t>Gazprom</t>
-  </si>
-  <si>
     <t>Spain</t>
   </si>
   <si>
-    <t>Barcelona LNG terminal</t>
-  </si>
-  <si>
     <t>Barcelona</t>
   </si>
   <si>
     <t>enagas</t>
   </si>
   <si>
-    <t>Bilbao LNG terminal</t>
-  </si>
-  <si>
     <t>Bilbao</t>
   </si>
   <si>
     <t>BBG</t>
   </si>
   <si>
-    <t>Cartagena LNG terminal</t>
-  </si>
-  <si>
     <t>Cartagena</t>
   </si>
   <si>
-    <t>El Musel LNG terminal</t>
-  </si>
-  <si>
     <t>Gijón (Musel)</t>
   </si>
   <si>
-    <t>Huelva LNG terminal</t>
-  </si>
-  <si>
     <t>Huelva</t>
   </si>
   <si>
-    <t>Mugardos LNG terminal</t>
-  </si>
-  <si>
     <t>Mugardos</t>
   </si>
   <si>
     <t>reganosa</t>
   </si>
   <si>
-    <t>Sagunto LNG terminal</t>
-  </si>
-  <si>
     <t>Sagunto</t>
   </si>
   <si>
@@ -322,45 +254,30 @@
     <t>Turkey</t>
   </si>
   <si>
-    <t>Aliga Etki LNG terminal</t>
-  </si>
-  <si>
     <t>Aliga Etki</t>
   </si>
   <si>
     <t>etklliman</t>
   </si>
   <si>
-    <t>Aliga Izmir LNG terminal</t>
-  </si>
-  <si>
     <t>Aliga Izmir</t>
   </si>
   <si>
     <t>EgeGaz</t>
   </si>
   <si>
-    <t>Dörtyol LNG terminal</t>
-  </si>
-  <si>
     <t>Dörtyol</t>
   </si>
   <si>
     <t>botgas</t>
   </si>
   <si>
-    <t>Marmara Ereglisi LNG terminal</t>
-  </si>
-  <si>
     <t>Marmara Ereglisi</t>
   </si>
   <si>
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>Grain LNG terminal</t>
-  </si>
-  <si>
     <t>Isle of Grain</t>
   </si>
   <si>
@@ -382,18 +299,12 @@
     <t>Cyprus</t>
   </si>
   <si>
-    <t>Vasiliko LNG terminal</t>
-  </si>
-  <si>
     <t xml:space="preserve">Vasiliko </t>
   </si>
   <si>
     <t>ETYFA</t>
   </si>
   <si>
-    <t>Alexandroupolis LNG terminal</t>
-  </si>
-  <si>
     <t>Alexandroupolis</t>
   </si>
   <si>
@@ -403,9 +314,6 @@
     <t>Albania</t>
   </si>
   <si>
-    <t>Vlora LNG terminal</t>
-  </si>
-  <si>
     <t>Vlora</t>
   </si>
   <si>
@@ -418,18 +326,12 @@
     <t>Estonia</t>
   </si>
   <si>
-    <t>Paldiski LNG terminal</t>
-  </si>
-  <si>
     <t>Paldiski</t>
   </si>
   <si>
     <t>Alexela</t>
   </si>
   <si>
-    <t>Tallinn LNG terminal</t>
-  </si>
-  <si>
     <t>Tallinn (Muuga)</t>
   </si>
   <si>
@@ -442,15 +344,9 @@
     <t>Exemplar FSRU</t>
   </si>
   <si>
-    <t>Inkoo</t>
-  </si>
-  <si>
     <t>gasgrid fortum</t>
   </si>
   <si>
-    <t>Le Havre LNG terminal</t>
-  </si>
-  <si>
     <t>Le Havre</t>
   </si>
   <si>
@@ -460,36 +356,24 @@
     <t>Germany</t>
   </si>
   <si>
-    <t>Brunsbüttel LNG terminal</t>
-  </si>
-  <si>
     <t>Brunsbüttel</t>
   </si>
   <si>
     <t>gasunte</t>
   </si>
   <si>
-    <t>Lubmin LNG terminal</t>
-  </si>
-  <si>
     <t>Lubmin</t>
   </si>
   <si>
     <t>deutsche RaGas</t>
   </si>
   <si>
-    <t>Stade LNG terminal</t>
-  </si>
-  <si>
     <t>Stade</t>
   </si>
   <si>
     <t>Hanseatic Energy Hub</t>
   </si>
   <si>
-    <t>Wilhelmshaven LNG terminal</t>
-  </si>
-  <si>
     <t>Wilhelmshaven</t>
   </si>
   <si>
@@ -499,25 +383,19 @@
     <t>TES</t>
   </si>
   <si>
-    <t>Argo LNG terminal</t>
-  </si>
-  <si>
     <t>Argo</t>
   </si>
   <si>
     <t>Mediterranean Gas</t>
   </si>
   <si>
-    <t>Dioriga FSRU</t>
-  </si>
-  <si>
-    <t>Gulf of Corinth</t>
+    <t>Dioriga Gas (Corynth)</t>
   </si>
   <si>
     <t>Gioriga Gas</t>
   </si>
   <si>
-    <t>Thrace  FSRU</t>
+    <t>Thrace LNG Terminal</t>
   </si>
   <si>
     <t>gas trade</t>
@@ -529,34 +407,19 @@
     <t>Shannon LNG</t>
   </si>
   <si>
-    <t>Tarbert/Ballylongford</t>
-  </si>
-  <si>
     <t>shannon LNG</t>
   </si>
   <si>
-    <t>Mag Mell FSRU</t>
-  </si>
-  <si>
-    <t>Cork</t>
+    <t>Mag Mell</t>
   </si>
   <si>
     <t xml:space="preserve">Mag Mell </t>
   </si>
   <si>
-    <t>Porto Torres FSRU</t>
-  </si>
-  <si>
-    <t>Porto Torres</t>
-  </si>
-  <si>
-    <t>Die Schiffe werden zwischen den Regasifizierungsterminals von Panigaglia (La Spezia) und Olt (Livorno) in Richtung der Fsru-Einheit pendeln, die im Industriehafen von Porto Torres installiert ist,</t>
-  </si>
-  <si>
-    <t>Ravenna FSRU</t>
-  </si>
-  <si>
-    <t>Ravenna</t>
+    <t>FSRU 1 - SNAM</t>
+  </si>
+  <si>
+    <t>FSRU 2 - SNAM</t>
   </si>
   <si>
     <t>Porto Empedoche</t>
@@ -577,28 +440,16 @@
     <t>VIRSI</t>
   </si>
   <si>
-    <t>Morocco</t>
-  </si>
-  <si>
-    <t>Jorf Lasfar</t>
-  </si>
-  <si>
-    <t>Morocco FSRU</t>
-  </si>
-  <si>
     <t>Gdansk LNG</t>
   </si>
   <si>
-    <t>Gdansk</t>
-  </si>
-  <si>
     <t>GAZ system</t>
   </si>
   <si>
-    <t>Gulf of Saros FSRU</t>
-  </si>
-  <si>
     <t>Gulf of Saros</t>
+  </si>
+  <si>
+    <t>possible expansion</t>
   </si>
 </sst>
 </file>
@@ -609,22 +460,10 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -634,8 +473,8 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="64"/>
+      <sz val="10.5"/>
+      <color rgb="FF5F6368"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -645,24 +484,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor rgb="FFFFEB9C"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -674,35 +501,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
-    <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -928,16 +743,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K68"/>
+  <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.88671875" customWidth="1"/>
+    <col min="1" max="2" width="12.88671875" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="5" width="18.109375" customWidth="1"/>
     <col min="6" max="6" width="27.44140625" bestFit="1" customWidth="1"/>
@@ -977,15 +791,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="13.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
       </c>
       <c r="D2" s="1">
         <v>3.22241</v>
@@ -994,13 +805,13 @@
         <v>51.353000000000002</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
       </c>
       <c r="I2" s="2">
         <v>11400000000</v>
@@ -1013,11 +824,8 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
       </c>
       <c r="D3" s="1">
         <v>3.22241</v>
@@ -1026,13 +834,13 @@
         <v>51.353000000000002</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I3" s="2">
         <v>3900000000</v>
@@ -1045,11 +853,8 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
       </c>
       <c r="D4" s="1">
         <v>3.22241</v>
@@ -1058,13 +863,13 @@
         <v>51.353000000000002</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I4" s="2">
         <v>1800000000</v>
@@ -1075,13 +880,10 @@
     </row>
     <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
       </c>
       <c r="D5" s="1">
         <v>14.6</v>
@@ -1090,13 +892,13 @@
         <v>45.066667000000002</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I5" s="2">
         <v>2600000000</v>
@@ -1107,13 +909,10 @@
     </row>
     <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
       </c>
       <c r="D6" s="1">
         <v>14.6</v>
@@ -1122,13 +921,13 @@
         <v>45.066668</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I6" s="2">
         <v>2600000000</v>
@@ -1137,30 +936,27 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2.1965300000000001</v>
+      </c>
+      <c r="E7" s="3">
+        <v>51.033610000000003</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1">
-        <v>2.1965300000000001</v>
-      </c>
-      <c r="E7" s="1">
-        <v>51.033610000000003</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s">
-        <v>25</v>
       </c>
       <c r="I7" s="2">
         <v>13000000000</v>
@@ -1171,13 +967,10 @@
     </row>
     <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1">
         <v>4.9010199999999999</v>
@@ -1186,13 +979,13 @@
         <v>43.419629999999998</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I8" s="2">
         <v>8500000000</v>
@@ -1203,13 +996,10 @@
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1">
         <v>4.9010199999999999</v>
@@ -1218,13 +1008,13 @@
         <v>43.419629999999998</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I9" s="2">
         <v>1500000000</v>
@@ -1235,13 +1025,10 @@
     </row>
     <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1">
         <v>4.9010199999999999</v>
@@ -1250,13 +1037,13 @@
         <v>43.419629999999998</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I10" s="2">
         <v>2000000000</v>
@@ -1267,13 +1054,10 @@
     </row>
     <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1">
         <v>4.9010199999999999</v>
@@ -1282,13 +1066,13 @@
         <v>43.419629999999998</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="I11" s="2">
         <v>1500000000</v>
@@ -1299,13 +1083,10 @@
     </row>
     <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1">
         <v>-2.1427800000000001</v>
@@ -1314,13 +1095,13 @@
         <v>47.302959999999999</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="I12" s="2">
         <v>10000000000</v>
@@ -1331,28 +1112,25 @@
     </row>
     <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1">
         <v>23.4023</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H13" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I13" s="2">
         <v>7000000000</v>
@@ -1363,28 +1141,28 @@
     </row>
     <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E14" s="1">
         <v>43.644444</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H14" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="I14" s="2">
         <v>3550000000</v>
@@ -1395,28 +1173,28 @@
     </row>
     <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E15" s="1">
         <v>43.644444999999997</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H15" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="I15" s="2">
         <v>1190000000</v>
@@ -1425,18 +1203,15 @@
         <v>2013</v>
       </c>
       <c r="K15" t="s">
-        <v>45</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D16" s="1">
         <v>9.8308700000000009</v>
@@ -1445,13 +1220,13 @@
         <v>44.074280000000002</v>
       </c>
       <c r="F16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H16" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I16" s="2">
         <v>3400000000</v>
@@ -1462,13 +1237,10 @@
     </row>
     <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D17" s="1">
         <v>12.586111000000001</v>
@@ -1477,13 +1249,13 @@
         <v>45.091667000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H17" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="I17" s="2">
         <v>9000000000</v>
@@ -1494,13 +1266,10 @@
     </row>
     <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D18" s="1">
         <v>21.137619999999998</v>
@@ -1509,13 +1278,13 @@
         <v>55.66451</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H18" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I18" s="2">
         <v>4000000000</v>
@@ -1526,13 +1295,10 @@
     </row>
     <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D19" s="1">
         <v>14.5542</v>
@@ -1541,13 +1307,13 @@
         <v>35.8277</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="G19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="I19" s="2">
         <v>700000000</v>
@@ -1558,13 +1324,13 @@
     </row>
     <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D20" s="1">
         <v>4.0688890000000004</v>
@@ -1573,13 +1339,13 @@
         <v>51.971111000000001</v>
       </c>
       <c r="F20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H20" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="I20" s="2">
         <v>12000000000</v>
@@ -1590,13 +1356,13 @@
     </row>
     <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D21" s="1">
         <v>4.0688890000000004</v>
@@ -1605,13 +1371,13 @@
         <v>51.971111000000001</v>
       </c>
       <c r="F21" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H21" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="I21" s="2">
         <v>4000000000</v>
@@ -1619,19 +1385,16 @@
       <c r="J21">
         <v>2011</v>
       </c>
-      <c r="K21" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D22" s="1">
         <v>4.0688890000000004</v>
@@ -1640,13 +1403,13 @@
         <v>51.971111000000001</v>
       </c>
       <c r="F22" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H22" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="I22" s="2">
         <v>1500000000</v>
@@ -1657,13 +1420,13 @@
     </row>
     <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D23" s="1">
         <v>4.0688890000000004</v>
@@ -1672,13 +1435,13 @@
         <v>51.971111000000001</v>
       </c>
       <c r="F23" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="G23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H23" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="I23" s="2">
         <v>2500000000</v>
@@ -1689,13 +1452,13 @@
     </row>
     <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D24" s="1">
         <v>6.8330976999999997</v>
@@ -1704,13 +1467,13 @@
         <v>53.435648700000002</v>
       </c>
       <c r="F24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H24" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="I24" s="2">
         <v>8000000000</v>
@@ -1721,13 +1484,10 @@
     </row>
     <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="D25" s="1">
         <v>14.294722</v>
@@ -1736,13 +1496,13 @@
         <v>53.909166999999997</v>
       </c>
       <c r="F25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H25" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="I25" s="2">
         <v>6200000000</v>
@@ -1753,13 +1513,10 @@
     </row>
     <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="D26" s="1">
         <v>14.294722</v>
@@ -1768,13 +1525,13 @@
         <v>53.909166999999997</v>
       </c>
       <c r="F26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H26" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="I26" s="2">
         <v>2100000000</v>
@@ -1785,13 +1542,10 @@
     </row>
     <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>72</v>
-      </c>
-      <c r="B27" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="D27" s="1">
         <v>-8.8435000000000006</v>
@@ -1800,13 +1554,13 @@
         <v>37.941899999999997</v>
       </c>
       <c r="F27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H27" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="I27" s="2">
         <v>7600000000</v>
@@ -1816,401 +1570,362 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="4">
-        <v>20.362926099999999</v>
-      </c>
-      <c r="E28" s="4">
-        <v>54.983699899999998</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="I28" s="5">
-        <v>3700000000</v>
-      </c>
-      <c r="J28" s="3">
-        <v>2019</v>
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2.1583000000000001</v>
+      </c>
+      <c r="E28" s="1">
+        <v>41.339399999999998</v>
+      </c>
+      <c r="F28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" t="s">
+        <v>62</v>
+      </c>
+      <c r="I28" s="2">
+        <v>17100000000</v>
+      </c>
+      <c r="J28">
+        <v>1968</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D29" s="1">
-        <v>2.1583000000000001</v>
+        <v>-3.0947300000000002</v>
       </c>
       <c r="E29" s="1">
-        <v>41.339399999999998</v>
+        <v>43.361199999999997</v>
       </c>
       <c r="F29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H29" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="I29" s="2">
-        <v>17100000000</v>
+        <v>7000000000</v>
       </c>
       <c r="J29">
-        <v>1968</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="C30" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="D30" s="1">
-        <v>-3.0947300000000002</v>
+        <v>-0.95950000000000002</v>
       </c>
       <c r="E30" s="1">
-        <v>43.361199999999997</v>
+        <v>37.574570000000001</v>
       </c>
       <c r="F30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H30" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="I30" s="2">
-        <v>7000000000</v>
+        <v>11800000000</v>
       </c>
       <c r="J30">
-        <v>2003</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>80</v>
-      </c>
-      <c r="B31" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="D31" s="1">
-        <v>-0.95950000000000002</v>
+        <v>-5.6933999999999996</v>
       </c>
       <c r="E31" s="1">
-        <v>37.574570000000001</v>
+        <v>43.569600000000001</v>
       </c>
       <c r="F31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H31" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="I31" s="2">
-        <v>11800000000</v>
+        <v>7000000000</v>
       </c>
       <c r="J31">
-        <v>1989</v>
+        <v>2012</v>
+      </c>
+      <c r="K31">
+        <v>-2023</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D32" s="1">
-        <v>-5.6933999999999996</v>
+        <v>-6.9109999999999996</v>
       </c>
       <c r="E32" s="1">
-        <v>43.569600000000001</v>
+        <v>37.173549999999999</v>
       </c>
       <c r="F32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H32" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="I32" s="2">
-        <v>7000000000</v>
+        <v>11800000000</v>
       </c>
       <c r="J32">
-        <v>2012</v>
-      </c>
-      <c r="K32">
-        <v>-2023</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="D33" s="1">
-        <v>-6.9109999999999996</v>
+        <v>-8.2394999999999996</v>
       </c>
       <c r="E33" s="1">
-        <v>37.173549999999999</v>
+        <v>43.461300000000001</v>
       </c>
       <c r="F33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H33" t="s">
-        <v>83</v>
-      </c>
-      <c r="I33" s="2">
-        <v>11800000000</v>
+        <v>69</v>
+      </c>
+      <c r="I33" s="4">
+        <v>3600000000</v>
       </c>
       <c r="J33">
-        <v>1988</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>80</v>
-      </c>
-      <c r="B34" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="D34" s="1">
-        <v>-8.2394999999999996</v>
+        <v>-0.2152</v>
       </c>
       <c r="E34" s="1">
-        <v>43.461300000000001</v>
+        <v>39.632899999999999</v>
       </c>
       <c r="F34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H34" t="s">
-        <v>95</v>
-      </c>
-      <c r="I34" s="6">
-        <v>3600000000</v>
+        <v>71</v>
+      </c>
+      <c r="I34" s="4">
+        <v>8800000000</v>
       </c>
       <c r="J34">
-        <v>2007</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>80</v>
-      </c>
-      <c r="B35" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="C35" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="D35" s="1">
-        <v>-0.2152</v>
+        <v>27.129000000000001</v>
       </c>
       <c r="E35" s="1">
-        <v>39.632899999999999</v>
+        <v>38.421999999999997</v>
       </c>
       <c r="F35" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H35" t="s">
-        <v>98</v>
-      </c>
-      <c r="I35" s="6">
-        <v>8800000000</v>
+        <v>74</v>
+      </c>
+      <c r="I35" s="4">
+        <v>7300000000</v>
       </c>
       <c r="J35">
-        <v>2006</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>99</v>
-      </c>
-      <c r="B36" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="C36" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="D36" s="1">
-        <v>27.129000000000001</v>
+        <v>26.970278</v>
       </c>
       <c r="E36" s="1">
-        <v>38.421999999999997</v>
+        <v>38.795000000000002</v>
       </c>
       <c r="F36" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H36" t="s">
-        <v>102</v>
-      </c>
-      <c r="I36" s="6">
-        <v>7300000000</v>
+        <v>76</v>
+      </c>
+      <c r="I36" s="4">
+        <v>13800000000</v>
       </c>
       <c r="J36">
-        <v>2016</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>99</v>
-      </c>
-      <c r="B37" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="C37" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="D37" s="1">
-        <v>26.970278</v>
+        <v>36.131414700000001</v>
       </c>
       <c r="E37" s="1">
-        <v>38.795000000000002</v>
+        <v>36.855579300000002</v>
       </c>
       <c r="F37" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H37" t="s">
-        <v>105</v>
-      </c>
-      <c r="I37" s="6">
-        <v>13800000000</v>
+        <v>78</v>
+      </c>
+      <c r="I37" s="4">
+        <v>9700000000</v>
       </c>
       <c r="J37">
-        <v>2006</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>99</v>
-      </c>
-      <c r="B38" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="C38" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="D38" s="1">
-        <v>36.131414700000001</v>
+        <v>27.955278</v>
       </c>
       <c r="E38" s="1">
-        <v>36.855579300000002</v>
+        <v>40.969721999999997</v>
       </c>
       <c r="F38" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H38" t="s">
-        <v>108</v>
-      </c>
-      <c r="I38" s="6">
-        <v>9700000000</v>
+        <v>78</v>
+      </c>
+      <c r="I38" s="4">
+        <v>12800000000</v>
       </c>
       <c r="J38">
-        <v>2018</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>99</v>
-      </c>
-      <c r="B39" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="C39" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="D39" s="1">
-        <v>27.955278</v>
+        <v>0.67986999999999997</v>
       </c>
       <c r="E39" s="1">
-        <v>40.969721999999997</v>
+        <v>51.451070000000001</v>
       </c>
       <c r="F39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H39" t="s">
-        <v>108</v>
-      </c>
-      <c r="I39" s="6">
-        <v>12800000000</v>
+        <v>82</v>
+      </c>
+      <c r="I39" s="4">
+        <v>19500000000</v>
       </c>
       <c r="J39">
-        <v>1994</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>111</v>
-      </c>
-      <c r="B40" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="C40" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="D40" s="1">
         <v>0.67986999999999997</v>
@@ -2219,62 +1934,56 @@
         <v>51.451070000000001</v>
       </c>
       <c r="F40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G40" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H40" t="s">
-        <v>114</v>
-      </c>
-      <c r="I40" s="6">
-        <v>19500000000</v>
+        <v>82</v>
+      </c>
+      <c r="I40" s="4">
+        <v>5000000000</v>
       </c>
       <c r="J40">
-        <v>2005</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>111</v>
-      </c>
-      <c r="B41" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="C41" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="D41" s="1">
-        <v>0.67986999999999997</v>
+        <v>-4.9977400000000003</v>
       </c>
       <c r="E41" s="1">
-        <v>51.451070000000001</v>
+        <v>51.704529999999998</v>
       </c>
       <c r="F41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G41" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H41" t="s">
-        <v>114</v>
-      </c>
-      <c r="I41" s="6">
-        <v>5000000000</v>
+        <v>84</v>
+      </c>
+      <c r="I41" s="4">
+        <v>7600000000</v>
       </c>
       <c r="J41">
-        <v>2025</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>111</v>
-      </c>
-      <c r="B42" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="C42" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="D42" s="1">
         <v>-4.9977400000000003</v>
@@ -2283,16 +1992,16 @@
         <v>51.704529999999998</v>
       </c>
       <c r="F42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H42" t="s">
-        <v>116</v>
-      </c>
-      <c r="I42" s="6">
-        <v>7600000000</v>
+        <v>86</v>
+      </c>
+      <c r="I42" s="4">
+        <v>21000000000</v>
       </c>
       <c r="J42">
         <v>2009</v>
@@ -2300,63 +2009,57 @@
     </row>
     <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>111</v>
-      </c>
-      <c r="B43" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="C43" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="D43" s="1">
-        <v>-4.9977400000000003</v>
+        <v>33.30104</v>
       </c>
       <c r="E43" s="1">
-        <v>51.704529999999998</v>
+        <v>34.727719999999998</v>
       </c>
       <c r="F43" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H43" t="s">
-        <v>118</v>
-      </c>
-      <c r="I43" s="6">
-        <v>21000000000</v>
+        <v>89</v>
+      </c>
+      <c r="I43" s="4">
+        <v>2440000000</v>
       </c>
       <c r="J43">
-        <v>2009</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B44" t="s">
-        <v>120</v>
+        <v>28</v>
       </c>
       <c r="C44" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="D44" s="1">
-        <v>33.30104</v>
+        <v>25.842735999999999</v>
       </c>
       <c r="E44" s="1">
-        <v>34.727719999999998</v>
+        <v>40.774729999999998</v>
       </c>
       <c r="F44" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H44" t="s">
-        <v>122</v>
-      </c>
-      <c r="I44" s="6">
-        <v>2440000000</v>
+        <v>91</v>
+      </c>
+      <c r="I44" s="4">
+        <v>5500000000</v>
       </c>
       <c r="J44">
         <v>2023</v>
@@ -2364,31 +2067,28 @@
     </row>
     <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>34</v>
-      </c>
-      <c r="B45" t="s">
-        <v>123</v>
+        <v>92</v>
       </c>
       <c r="C45" t="s">
-        <v>124</v>
+        <v>93</v>
       </c>
       <c r="D45" s="1">
-        <v>25.842735999999999</v>
+        <v>19.480761000000001</v>
       </c>
       <c r="E45" s="1">
-        <v>40.774729999999998</v>
+        <v>40.449271000000003</v>
       </c>
       <c r="F45" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H45" t="s">
-        <v>125</v>
-      </c>
-      <c r="I45" s="6">
-        <v>5500000000</v>
+        <v>94</v>
+      </c>
+      <c r="I45" t="s">
+        <v>95</v>
       </c>
       <c r="J45">
         <v>2023</v>
@@ -2396,269 +2096,236 @@
     </row>
     <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>126</v>
-      </c>
-      <c r="B46" t="s">
-        <v>127</v>
+        <v>96</v>
       </c>
       <c r="C46" t="s">
-        <v>128</v>
+        <v>97</v>
       </c>
       <c r="D46" s="1">
-        <v>19.480761000000001</v>
+        <v>24.074940000000002</v>
       </c>
       <c r="E46" s="1">
-        <v>40.449271000000003</v>
+        <v>59.384450000000001</v>
       </c>
       <c r="F46" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H46" t="s">
-        <v>129</v>
-      </c>
-      <c r="I46" t="s">
-        <v>130</v>
+        <v>98</v>
+      </c>
+      <c r="I46" s="4">
+        <v>2500000000</v>
       </c>
       <c r="J46">
-        <v>2023</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>131</v>
-      </c>
-      <c r="B47" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="C47" t="s">
-        <v>133</v>
+        <v>99</v>
       </c>
       <c r="D47" s="1">
-        <v>24.074940000000002</v>
+        <v>25.0045</v>
       </c>
       <c r="E47" s="1">
-        <v>59.384450000000001</v>
+        <v>59.506010000000003</v>
       </c>
       <c r="F47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H47" t="s">
-        <v>134</v>
-      </c>
-      <c r="I47" s="6">
-        <v>2500000000</v>
-      </c>
-      <c r="J47">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="I47" s="4">
+        <v>4000000000</v>
+      </c>
+      <c r="J47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>131</v>
-      </c>
-      <c r="B48" t="s">
-        <v>135</v>
+        <v>101</v>
       </c>
       <c r="C48" t="s">
-        <v>136</v>
-      </c>
-      <c r="D48" s="1">
-        <v>25.0045</v>
-      </c>
-      <c r="E48" s="1">
-        <v>59.506010000000003</v>
+        <v>102</v>
       </c>
       <c r="F48" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H48" t="s">
-        <v>137</v>
-      </c>
-      <c r="I48" s="6">
-        <v>4000000000</v>
-      </c>
-      <c r="J48" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="I48" s="4">
+        <v>5000000000</v>
+      </c>
+      <c r="J48">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>138</v>
-      </c>
-      <c r="B49" t="s">
-        <v>139</v>
+        <v>20</v>
       </c>
       <c r="C49" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
       <c r="D49" s="1">
-        <v>24.006440999999999</v>
+        <v>4.2958425760000002E-2</v>
       </c>
       <c r="E49" s="1">
-        <v>60.041103</v>
+        <v>49.462228393267502</v>
       </c>
       <c r="F49" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H49" t="s">
-        <v>141</v>
-      </c>
-      <c r="I49" s="6">
+        <v>105</v>
+      </c>
+      <c r="I49" t="s">
+        <v>95</v>
+      </c>
+      <c r="J49" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" t="s">
+        <v>107</v>
+      </c>
+      <c r="D50" s="1">
+        <v>8.9760945000000003</v>
+      </c>
+      <c r="E50" s="1">
+        <v>53.914000899999998</v>
+      </c>
+      <c r="F50" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" t="s">
+        <v>13</v>
+      </c>
+      <c r="H50" t="s">
+        <v>108</v>
+      </c>
+      <c r="I50" s="4">
         <v>5000000000</v>
       </c>
-      <c r="J49">
+      <c r="J50">
         <v>2023</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>22</v>
-      </c>
-      <c r="B50" t="s">
-        <v>142</v>
-      </c>
-      <c r="C50" t="s">
-        <v>143</v>
-      </c>
-      <c r="D50" s="1">
-        <v>4.2958425760000002E-2</v>
-      </c>
-      <c r="E50" s="1">
-        <v>49.462228393267502</v>
-      </c>
-      <c r="F50" t="s">
-        <v>20</v>
-      </c>
-      <c r="G50" t="s">
-        <v>14</v>
-      </c>
-      <c r="H50" t="s">
-        <v>144</v>
-      </c>
-      <c r="I50" t="s">
-        <v>130</v>
-      </c>
-      <c r="J50" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>145</v>
-      </c>
-      <c r="B51" t="s">
-        <v>146</v>
+        <v>106</v>
       </c>
       <c r="C51" t="s">
-        <v>147</v>
+        <v>109</v>
       </c>
       <c r="D51" s="1">
-        <v>8.9760945000000003</v>
+        <v>13.645319000000001</v>
       </c>
       <c r="E51" s="1">
-        <v>53.914000899999998</v>
+        <v>54.153331999999999</v>
       </c>
       <c r="F51" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H51" t="s">
-        <v>148</v>
-      </c>
-      <c r="I51" s="6">
-        <v>5000000000</v>
+        <v>110</v>
+      </c>
+      <c r="I51" s="4">
+        <v>4500000000</v>
       </c>
       <c r="J51">
         <v>2023</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>145</v>
-      </c>
-      <c r="B52" t="s">
-        <v>149</v>
+        <v>106</v>
       </c>
       <c r="C52" t="s">
-        <v>150</v>
+        <v>111</v>
       </c>
       <c r="D52" s="1">
-        <v>13.645319000000001</v>
+        <v>9.5103819999999999</v>
       </c>
       <c r="E52" s="1">
-        <v>54.153331999999999</v>
+        <v>53.652459</v>
       </c>
       <c r="F52" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H52" t="s">
-        <v>151</v>
-      </c>
-      <c r="I52" s="6">
-        <v>4500000000</v>
+        <v>112</v>
+      </c>
+      <c r="I52" s="4">
+        <v>12000000000</v>
       </c>
       <c r="J52">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" s="1">
+        <v>8.1333330000000004</v>
+      </c>
+      <c r="E53" s="1">
+        <v>53.516666999999998</v>
+      </c>
+      <c r="F53" t="s">
+        <v>18</v>
+      </c>
+      <c r="G53" t="s">
+        <v>13</v>
+      </c>
+      <c r="H53" t="s">
+        <v>114</v>
+      </c>
+      <c r="I53" s="4">
+        <v>7500000000</v>
+      </c>
+      <c r="J53">
         <v>2023</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>145</v>
-      </c>
-      <c r="B53" t="s">
-        <v>152</v>
-      </c>
-      <c r="C53" t="s">
-        <v>153</v>
-      </c>
-      <c r="D53" s="1">
-        <v>9.5103819999999999</v>
-      </c>
-      <c r="E53" s="1">
-        <v>53.652459</v>
-      </c>
-      <c r="F53" t="s">
-        <v>13</v>
-      </c>
-      <c r="G53" t="s">
-        <v>14</v>
-      </c>
-      <c r="H53" t="s">
-        <v>154</v>
-      </c>
-      <c r="I53" s="6">
-        <v>12000000000</v>
-      </c>
-      <c r="J53">
-        <v>2026</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>145</v>
-      </c>
-      <c r="B54" t="s">
-        <v>155</v>
+        <v>106</v>
       </c>
       <c r="C54" t="s">
-        <v>156</v>
+        <v>113</v>
       </c>
       <c r="D54" s="1">
         <v>8.1333330000000004</v>
@@ -2667,445 +2334,319 @@
         <v>53.516666999999998</v>
       </c>
       <c r="F54" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G54" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H54" t="s">
-        <v>157</v>
-      </c>
-      <c r="I54" s="6">
-        <v>7500000000</v>
+        <v>115</v>
+      </c>
+      <c r="I54" s="4">
+        <v>2200000000</v>
       </c>
       <c r="J54">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" t="s">
+        <v>116</v>
+      </c>
+      <c r="D55" s="1">
+        <v>22.932490399999999</v>
+      </c>
+      <c r="E55" s="1">
+        <v>39.351264399999998</v>
+      </c>
+      <c r="F55" t="s">
+        <v>18</v>
+      </c>
+      <c r="G55" t="s">
+        <v>13</v>
+      </c>
+      <c r="H55" t="s">
+        <v>117</v>
+      </c>
+      <c r="I55" s="4">
+        <v>5200000000</v>
+      </c>
+      <c r="J55">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" t="s">
+        <v>118</v>
+      </c>
+      <c r="D56" s="1">
+        <v>23.063538999999999</v>
+      </c>
+      <c r="E56" s="1">
+        <v>37.910919999999997</v>
+      </c>
+      <c r="F56" t="s">
+        <v>18</v>
+      </c>
+      <c r="G56" t="s">
+        <v>13</v>
+      </c>
+      <c r="H56" t="s">
+        <v>119</v>
+      </c>
+      <c r="I56" s="4">
+        <v>3000000000</v>
+      </c>
+      <c r="J56">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57" t="s">
+        <v>120</v>
+      </c>
+      <c r="D57" s="1">
+        <v>25.718754000000001</v>
+      </c>
+      <c r="E57" s="1">
+        <v>40.748353999999999</v>
+      </c>
+      <c r="F57" t="s">
+        <v>18</v>
+      </c>
+      <c r="G57" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" t="s">
+        <v>121</v>
+      </c>
+      <c r="I57" s="4">
+        <v>5500000000</v>
+      </c>
+      <c r="J57" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58" t="s">
+        <v>123</v>
+      </c>
+      <c r="D58" s="1">
+        <v>-9.4424600000000005</v>
+      </c>
+      <c r="E58" s="1">
+        <v>52.58099</v>
+      </c>
+      <c r="F58" t="s">
+        <v>18</v>
+      </c>
+      <c r="G58" t="s">
+        <v>13</v>
+      </c>
+      <c r="H58" t="s">
+        <v>124</v>
+      </c>
+      <c r="I58" s="4">
+        <v>7800000000</v>
+      </c>
+      <c r="J58" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>122</v>
+      </c>
+      <c r="C59" t="s">
+        <v>125</v>
+      </c>
+      <c r="D59" s="1">
+        <v>-8.0456190000000003</v>
+      </c>
+      <c r="E59" s="1">
+        <v>51.264274</v>
+      </c>
+      <c r="F59" t="s">
+        <v>18</v>
+      </c>
+      <c r="G59" t="s">
+        <v>13</v>
+      </c>
+      <c r="H59" t="s">
+        <v>126</v>
+      </c>
+      <c r="I59" s="4">
+        <v>2600000000</v>
+      </c>
+      <c r="J59">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>32</v>
+      </c>
+      <c r="C60" t="s">
+        <v>127</v>
+      </c>
+      <c r="F60" t="s">
+        <v>18</v>
+      </c>
+      <c r="G60" t="s">
+        <v>13</v>
+      </c>
+      <c r="H60" t="s">
+        <v>39</v>
+      </c>
+      <c r="I60" s="4">
+        <v>5000000000</v>
+      </c>
+      <c r="J60">
         <v>2023</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>145</v>
-      </c>
-      <c r="B55" t="s">
-        <v>155</v>
-      </c>
-      <c r="C55" t="s">
-        <v>156</v>
-      </c>
-      <c r="D55" s="1">
-        <v>8.1333330000000004</v>
-      </c>
-      <c r="E55" s="1">
-        <v>53.516666999999998</v>
-      </c>
-      <c r="F55" t="s">
-        <v>20</v>
-      </c>
-      <c r="G55" t="s">
-        <v>16</v>
-      </c>
-      <c r="H55" t="s">
-        <v>158</v>
-      </c>
-      <c r="I55" s="6">
-        <v>2200000000</v>
-      </c>
-      <c r="J55">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>32</v>
+      </c>
+      <c r="C61" t="s">
+        <v>128</v>
+      </c>
+      <c r="F61" t="s">
+        <v>18</v>
+      </c>
+      <c r="G61" t="s">
+        <v>13</v>
+      </c>
+      <c r="H61" t="s">
+        <v>39</v>
+      </c>
+      <c r="I61" s="4">
+        <v>5000000000</v>
+      </c>
+      <c r="J61">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>32</v>
+      </c>
+      <c r="C62" t="s">
+        <v>129</v>
+      </c>
+      <c r="D62" s="1">
+        <v>13.537739999999999</v>
+      </c>
+      <c r="E62" s="1">
+        <v>37.282969999999999</v>
+      </c>
+      <c r="F62" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H62" t="s">
+        <v>130</v>
+      </c>
+      <c r="I62" s="4">
+        <v>8000000000</v>
+      </c>
+      <c r="J62">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>131</v>
+      </c>
+      <c r="C63" t="s">
+        <v>132</v>
+      </c>
+      <c r="D63" s="1">
+        <v>24.367000000000001</v>
+      </c>
+      <c r="E63" s="1">
+        <v>57.314999999999998</v>
+      </c>
+      <c r="F63" t="s">
+        <v>133</v>
+      </c>
+      <c r="G63" t="s">
+        <v>13</v>
+      </c>
+      <c r="H63" t="s">
+        <v>134</v>
+      </c>
+      <c r="I63" s="4">
+        <v>1500000000</v>
+      </c>
+      <c r="J63">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>54</v>
+      </c>
+      <c r="C64" t="s">
+        <v>135</v>
+      </c>
+      <c r="D64" s="1">
+        <v>18.716445</v>
+      </c>
+      <c r="E64" s="1">
+        <v>54.407321000000003</v>
+      </c>
+      <c r="F64" t="s">
+        <v>18</v>
+      </c>
+      <c r="G64" t="s">
+        <v>13</v>
+      </c>
+      <c r="H64" t="s">
+        <v>136</v>
+      </c>
+      <c r="I64" s="4">
+        <v>6100000000</v>
+      </c>
+      <c r="J64">
         <v>2025</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>34</v>
-      </c>
-      <c r="B56" t="s">
-        <v>159</v>
-      </c>
-      <c r="C56" t="s">
-        <v>160</v>
-      </c>
-      <c r="D56" s="1">
-        <v>22.932490399999999</v>
-      </c>
-      <c r="E56" s="1">
-        <v>39.351264399999998</v>
-      </c>
-      <c r="F56" t="s">
-        <v>20</v>
-      </c>
-      <c r="G56" t="s">
-        <v>14</v>
-      </c>
-      <c r="H56" t="s">
-        <v>161</v>
-      </c>
-      <c r="I56" s="6">
-        <v>5200000000</v>
-      </c>
-      <c r="J56">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>34</v>
-      </c>
-      <c r="B57" t="s">
-        <v>162</v>
-      </c>
-      <c r="C57" t="s">
-        <v>163</v>
-      </c>
-      <c r="D57" s="1">
-        <v>23.063538999999999</v>
-      </c>
-      <c r="E57" s="1">
-        <v>37.910919999999997</v>
-      </c>
-      <c r="F57" t="s">
-        <v>20</v>
-      </c>
-      <c r="G57" t="s">
-        <v>14</v>
-      </c>
-      <c r="H57" t="s">
-        <v>164</v>
-      </c>
-      <c r="I57" s="6">
-        <v>3000000000</v>
-      </c>
-      <c r="J57">
-        <v>2026</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>34</v>
-      </c>
-      <c r="B58" t="s">
-        <v>165</v>
-      </c>
-      <c r="C58" t="s">
-        <v>124</v>
-      </c>
-      <c r="D58" s="1">
-        <v>25.718754000000001</v>
-      </c>
-      <c r="E58" s="1">
-        <v>40.748353999999999</v>
-      </c>
-      <c r="F58" t="s">
-        <v>20</v>
-      </c>
-      <c r="G58" t="s">
-        <v>14</v>
-      </c>
-      <c r="H58" t="s">
-        <v>166</v>
-      </c>
-      <c r="I58" s="6">
-        <v>5500000000</v>
-      </c>
-      <c r="J58" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>167</v>
-      </c>
-      <c r="B59" t="s">
-        <v>168</v>
-      </c>
-      <c r="C59" t="s">
-        <v>169</v>
-      </c>
-      <c r="D59" s="1">
-        <v>-9.4424600000000005</v>
-      </c>
-      <c r="E59" s="1">
-        <v>52.58099</v>
-      </c>
-      <c r="F59" t="s">
-        <v>20</v>
-      </c>
-      <c r="G59" t="s">
-        <v>14</v>
-      </c>
-      <c r="H59" t="s">
-        <v>170</v>
-      </c>
-      <c r="I59" s="6">
-        <v>7800000000</v>
-      </c>
-      <c r="J59" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>167</v>
-      </c>
-      <c r="B60" t="s">
-        <v>171</v>
-      </c>
-      <c r="C60" t="s">
-        <v>172</v>
-      </c>
-      <c r="D60" s="1">
-        <v>-8.0456190000000003</v>
-      </c>
-      <c r="E60" s="1">
-        <v>51.264274</v>
-      </c>
-      <c r="F60" t="s">
-        <v>20</v>
-      </c>
-      <c r="G60" t="s">
-        <v>14</v>
-      </c>
-      <c r="H60" t="s">
-        <v>173</v>
-      </c>
-      <c r="I60" s="6">
-        <v>2600000000</v>
-      </c>
-      <c r="J60">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="D61" s="8">
-        <v>8.3957188499999997</v>
-      </c>
-      <c r="E61" s="8">
-        <v>40.846639830000001</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G61" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H61" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="I61" s="9">
-        <v>5000000000</v>
-      </c>
-      <c r="J61" s="7">
-        <v>2023</v>
-      </c>
-      <c r="K61" s="10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G62" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H62" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="I62" s="9">
-        <v>5000000000</v>
-      </c>
-      <c r="J62" s="7">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>39</v>
-      </c>
-      <c r="B63" t="s">
-        <v>179</v>
-      </c>
-      <c r="C63" t="s">
-        <v>179</v>
-      </c>
-      <c r="D63" s="1">
-        <v>13.537739999999999</v>
-      </c>
-      <c r="E63" s="1">
-        <v>37.282969999999999</v>
-      </c>
-      <c r="F63" t="s">
-        <v>13</v>
-      </c>
-      <c r="G63" t="s">
-        <v>14</v>
-      </c>
-      <c r="H63" t="s">
-        <v>180</v>
-      </c>
-      <c r="I63" s="6">
-        <v>8000000000</v>
-      </c>
-      <c r="J63">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>181</v>
-      </c>
-      <c r="B64" t="s">
-        <v>182</v>
-      </c>
-      <c r="C64" t="s">
-        <v>182</v>
-      </c>
-      <c r="D64" s="1">
-        <v>24.367000000000001</v>
-      </c>
-      <c r="E64" s="1">
-        <v>57.314999999999998</v>
-      </c>
-      <c r="F64" t="s">
-        <v>183</v>
-      </c>
-      <c r="G64" t="s">
-        <v>14</v>
-      </c>
-      <c r="H64" t="s">
-        <v>184</v>
-      </c>
-      <c r="I64" s="6">
-        <v>1500000000</v>
-      </c>
-      <c r="J64">
-        <v>2023</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>185</v>
-      </c>
-      <c r="B65" t="s">
-        <v>186</v>
+        <v>72</v>
       </c>
       <c r="C65" t="s">
-        <v>186</v>
+        <v>137</v>
       </c>
       <c r="D65" s="1">
-        <v>-8.6202799999999993</v>
+        <v>26.412033999999998</v>
       </c>
       <c r="E65" s="1">
-        <v>33.1267</v>
+        <v>40.594648999999997</v>
       </c>
       <c r="F65" t="s">
-        <v>13</v>
-      </c>
-      <c r="G65" t="s">
-        <v>14</v>
-      </c>
-      <c r="I65" s="6">
-        <v>5000000000</v>
-      </c>
-      <c r="J65" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>185</v>
-      </c>
-      <c r="B66" t="s">
-        <v>187</v>
-      </c>
-      <c r="C66" t="s">
-        <v>187</v>
-      </c>
-      <c r="F66" t="s">
-        <v>20</v>
-      </c>
-      <c r="G66" t="s">
-        <v>14</v>
-      </c>
-      <c r="I66" s="6">
-        <v>3000000000</v>
-      </c>
-      <c r="J66">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="15" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>68</v>
-      </c>
-      <c r="B67" t="s">
-        <v>188</v>
-      </c>
-      <c r="C67" t="s">
-        <v>189</v>
-      </c>
-      <c r="D67" s="1">
-        <v>18.716445</v>
-      </c>
-      <c r="E67" s="1">
-        <v>54.407321000000003</v>
-      </c>
-      <c r="F67" t="s">
-        <v>20</v>
-      </c>
-      <c r="G67" t="s">
-        <v>14</v>
-      </c>
-      <c r="H67" t="s">
-        <v>190</v>
-      </c>
-      <c r="I67" s="6">
-        <v>6100000000</v>
-      </c>
-      <c r="J67">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="15" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>99</v>
-      </c>
-      <c r="B68" t="s">
-        <v>191</v>
-      </c>
-      <c r="C68" t="s">
-        <v>192</v>
-      </c>
-      <c r="D68" s="1">
-        <v>26.412033999999998</v>
-      </c>
-      <c r="E68" s="1">
-        <v>40.594648999999997</v>
-      </c>
-      <c r="F68" t="s">
-        <v>20</v>
-      </c>
-      <c r="I68" s="6">
+        <v>18</v>
+      </c>
+      <c r="I65" s="4">
         <v>9700000000</v>
       </c>
-      <c r="J68">
+      <c r="J65">
         <v>2022</v>
       </c>
     </row>

</xml_diff>